<commit_message>
Changed all links to Ryzen 7000
</commit_message>
<xml_diff>
--- a/price_check.xlsx
+++ b/price_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\david\MyStuff\Docs\VSC_Projects\PriceCheck\PriceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA265B8C-BF61-4D8E-A717-93B847B99FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39671223-570D-4399-A6B8-00DA73F09847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="3060" windowWidth="23040" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1008" yWindow="1092" windowWidth="23040" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -34,13 +34,16 @@
     <t>date</t>
   </si>
   <si>
-    <t>pMark_AMD Ryzen 9 5900X</t>
-  </si>
-  <si>
-    <t>pMark_AMD Ryzen 7 5800X3D</t>
-  </si>
-  <si>
-    <t>pMark_AMD Ryzen 7 5800X</t>
+    <t>AMD Ryzen 5 7600X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 7700X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 7900X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 7950X</t>
   </si>
 </sst>
 </file>
@@ -408,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
@@ -439,13 +442,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>349</v>
+        <v>249.99</v>
       </c>
       <c r="C2">
-        <v>459.99</v>
+        <v>319.99</v>
       </c>
       <c r="D2" s="2">
-        <v>44994.432310071781</v>
+        <v>44999.415338126288</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -453,13 +456,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>323</v>
+        <v>344.99</v>
       </c>
       <c r="C3">
-        <v>434.99</v>
+        <v>444.99</v>
       </c>
       <c r="D3" s="2">
-        <v>44994.432310071781</v>
+        <v>44999.415338126288</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,13 +470,27 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>211.63</v>
+        <v>436.55</v>
       </c>
       <c r="C4">
-        <v>309.99</v>
+        <v>579.99</v>
       </c>
       <c r="D4" s="2">
-        <v>44994.432310071781</v>
+        <v>44999.415338126288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>599.99</v>
+      </c>
+      <c r="C5">
+        <v>759.99</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44999.415338126288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>